<commit_message>
updated timeline to include obejectives met
</commit_message>
<xml_diff>
--- a/01-planning/Literature Matrix .xlsx
+++ b/01-planning/Literature Matrix .xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuahellewell/Desktop/02-msc/01-modules/MSc Project - 771952/01-planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C808C4A0-05C0-0E49-B6BD-FE81EF9367F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E25008-8A6E-764F-8C0A-8181C3A5D39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="21260" xr2:uid="{781DB44C-E4D8-9E42-A974-8BBF4B8E3D6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -572,10 +572,10 @@
     <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -914,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6962E3-151D-1D4A-A12F-943D212A2AA3}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
@@ -927,7 +927,7 @@
     <col min="4" max="5" width="10.83203125" style="4"/>
     <col min="6" max="6" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="107.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="108.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="72.6640625" style="4" customWidth="1"/>
     <col min="10" max="10" width="57.33203125" style="4" customWidth="1"/>
     <col min="11" max="11" width="25" style="4" customWidth="1"/>
@@ -1109,7 +1109,7 @@
       <c r="J5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>41</v>
       </c>
       <c r="L5" s="7" t="s">
@@ -1119,7 +1119,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7" t="s">
@@ -1240,7 +1240,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="H11" s="10"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>

</xml_diff>

<commit_message>
added lit review & started abstract
</commit_message>
<xml_diff>
--- a/01-planning/Literature Matrix .xlsx
+++ b/01-planning/Literature Matrix .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuahellewell/Desktop/02-msc/01-modules/MSc Project - 771952/01-planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F930E4B2-D261-BD45-83AA-5E9758488FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEB5861-4D92-614A-9DE2-2723BB04E71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34480" yWindow="660" windowWidth="34160" windowHeight="27980" xr2:uid="{781DB44C-E4D8-9E42-A974-8BBF4B8E3D6B}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="68480" windowHeight="27980" xr2:uid="{781DB44C-E4D8-9E42-A974-8BBF4B8E3D6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -357,13 +357,6 @@
 Allows working with .stl , .ply and .obj</t>
   </si>
   <si>
-    <t>Parameterising aerodynamic shapes: B-splines, Bezier curves, FFD, class-shape transforms, Parsec and Bezier PARSEC.
-Computational cost greatly affected by compactness of design space.
-For 2D airfoilds - 10s of design variables. 
-For 3D - 100s of shape design variables for wing problems.
-PCA or SVD work for simple - but real world requires non-linearities.</t>
-  </si>
-  <si>
     <t>Deep Learning for ASO in 3D limited to dimensionality reduction with free-form deformation methods or 2D sketches that are subsequently stacked.
 None of the work with 3D meshes without externally partameterising their possible paths of deform or relying on intermediate reps.
 Convolutions are not trivial in non-euclidean domain,.
@@ -384,6 +377,14 @@
   </si>
   <si>
     <t>Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GA
+Shape Optimisation
+Pareto front.
+Geometric Deep Learning.
+Variational Bayesian methods.
+Reparameterisation trick </t>
   </si>
   <si>
     <r>
@@ -417,15 +418,19 @@
       </rPr>
       <t xml:space="preserve">
 Scale the node features by normalising mesh at 0,0,0 and scale to fit in cube with unitary edges.
-VAE can produce near original and new content with low dimensional vector.</t>
+VAE can produce near original and new content with low dimensional vector.
+VAE regularised through Variational Bayesian methods to ensure latent space has good properies.
+Spectral convolutions Chebyshev polynomial filters. 
+KL divergence to make distribution of encoder close to multivariate normal distribution.</t>
     </r>
   </si>
   <si>
-    <t>GA
-Shape Optimisation
-Pareto front.
-Geometric Deep Learning.
-Variational Bayesian methods.</t>
+    <t>Parameterising aerodynamic shapes: B-splines, Bezier curves, FFD, class-shape transforms, Parsec and Bezier PARSEC.
+Computational cost greatly affected by compactness of design space.
+For 2D airfoilds - 10s of design variables. 
+For 3D - 100s of shape design variables for wing problems.
+PCA or SVD work for simple - but real world requires non-linearities.
+Default - set to 4 dimensions</t>
   </si>
 </sst>
 </file>
@@ -928,9 +933,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6962E3-151D-1D4A-A12F-943D212A2AA3}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,7 +953,7 @@
     <col min="11" max="11" width="57.33203125" style="4" customWidth="1"/>
     <col min="12" max="12" width="25" style="4" customWidth="1"/>
     <col min="13" max="13" width="22.6640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="49.33203125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="82.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -966,13 +971,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>12</v>
@@ -1010,7 +1015,7 @@
         <v>42583</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>
@@ -1186,7 +1191,7 @@
         <v>51</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="7">
         <v>2024</v>
@@ -1198,20 +1203,20 @@
         <v>53</v>
       </c>
       <c r="G7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>54</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M7" s="7"/>
       <c r="N7" s="7" t="s">

</xml_diff>